<commit_message>
More advanced R tutorial
</commit_message>
<xml_diff>
--- a/data/more_advanced_R_membrane_potential.xlsx
+++ b/data/more_advanced_R_membrane_potential.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Introduction.to.R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A916C240-128D-5C4D-8F63-7F427A2476CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464586D6-43C0-C845-B519-0283567B8683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{C7523A4D-158F-5A49-9F53-A6C39F973F82}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>Cell_type</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Sample10</t>
+  </si>
+  <si>
+    <t>Day_of_experiment</t>
   </si>
 </sst>
 </file>
@@ -436,18 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB0CA41-76FD-5941-BF56-57AC44AAF16A}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +464,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -474,8 +481,11 @@
       <c r="D2">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -488,8 +498,11 @@
       <c r="D3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -502,8 +515,11 @@
       <c r="D4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -516,8 +532,11 @@
       <c r="D5">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -530,8 +549,11 @@
       <c r="D6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -544,8 +566,11 @@
       <c r="D7">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -558,8 +583,11 @@
       <c r="D8">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -572,8 +600,11 @@
       <c r="D9">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -586,8 +617,11 @@
       <c r="D10">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -600,8 +634,11 @@
       <c r="D11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -614,8 +651,11 @@
       <c r="D12">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -628,8 +668,11 @@
       <c r="D13">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -642,8 +685,11 @@
       <c r="D14">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -656,8 +702,11 @@
       <c r="D15">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -670,8 +719,11 @@
       <c r="D16">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -684,8 +736,11 @@
       <c r="D17">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -698,8 +753,11 @@
       <c r="D18">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -712,8 +770,11 @@
       <c r="D19">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -726,8 +787,11 @@
       <c r="D20">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -739,6 +803,9 @@
       </c>
       <c r="D21">
         <v>2.5</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>